<commit_message>
added colors for xlsx
</commit_message>
<xml_diff>
--- a/data_collection/test.xlsx
+++ b/data_collection/test.xlsx
@@ -78,7 +78,7 @@
   <numFmts count="1">
     <numFmt formatCode="General" numFmtId="164"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <name val="Calibri"/>
       <charset val="1"/>
@@ -107,6 +107,12 @@
       <family val="2"/>
       <color rgb="FFC9211E"/>
       <sz val="11"/>
+    </font>
+    <font>
+      <color rgb="0000FF00"/>
+    </font>
+    <font>
+      <color rgb="00FF0000"/>
     </font>
   </fonts>
   <fills count="3">
@@ -140,7 +146,7 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
@@ -151,6 +157,12 @@
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="5" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="6" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -579,7 +591,7 @@
       <c r="E5" s="1" t="n">
         <v>0.1</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -599,7 +611,7 @@
       <c r="E6" s="1" t="n">
         <v>0.1152542372881356</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -619,7 +631,7 @@
       <c r="E7" s="1" t="n">
         <v>0.1305084745762712</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -639,7 +651,7 @@
       <c r="E8" s="1" t="n">
         <v>0.1457627118644068</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -659,7 +671,7 @@
       <c r="E9" s="1" t="n">
         <v>0.1610169491525424</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -679,7 +691,7 @@
       <c r="E10" s="1" t="n">
         <v>0.176271186440678</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -699,7 +711,7 @@
       <c r="E11" s="1" t="n">
         <v>0.1915254237288136</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -719,7 +731,7 @@
       <c r="E12" s="1" t="n">
         <v>0.2067796610169492</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -739,7 +751,7 @@
       <c r="E13" s="1" t="n">
         <v>0.2220338983050847</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -759,7 +771,7 @@
       <c r="E14" s="1" t="n">
         <v>0.2372881355932203</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -779,7 +791,7 @@
       <c r="E15" s="1" t="n">
         <v>0.2525423728813559</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F15" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -799,7 +811,7 @@
       <c r="E16" s="1" t="n">
         <v>0.2677966101694915</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F16" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -819,7 +831,7 @@
       <c r="E17" s="1" t="n">
         <v>0.2830508474576271</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F17" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -839,7 +851,7 @@
       <c r="E18" s="1" t="n">
         <v>0.2983050847457627</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="F18" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -859,7 +871,7 @@
       <c r="E19" s="1" t="n">
         <v>0.3135593220338984</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F19" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -879,7 +891,7 @@
       <c r="E20" s="1" t="n">
         <v>0.3288135593220339</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="F20" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -899,7 +911,7 @@
       <c r="E21" s="1" t="n">
         <v>0.3440677966101695</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="F21" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -919,7 +931,7 @@
       <c r="E22" s="1" t="n">
         <v>0.3593220338983051</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F22" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -939,7 +951,7 @@
       <c r="E23" s="1" t="n">
         <v>0.3745762711864407</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="F23" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -959,7 +971,7 @@
       <c r="E24" s="1" t="n">
         <v>0.3898305084745763</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="F24" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -979,7 +991,7 @@
       <c r="E25" s="1" t="n">
         <v>0.4050847457627119</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="F25" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -999,7 +1011,7 @@
       <c r="E26" s="1" t="n">
         <v>0.4203389830508475</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="F26" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1019,7 +1031,7 @@
       <c r="E27" s="1" t="n">
         <v>0.4355932203389831</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="F27" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1039,7 +1051,7 @@
       <c r="E28" s="1" t="n">
         <v>0.4508474576271186</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="F28" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1059,7 +1071,7 @@
       <c r="E29" s="1" t="n">
         <v>0.4661016949152542</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="F29" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1079,7 +1091,7 @@
       <c r="E30" s="1" t="n">
         <v>0.4813559322033899</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="F30" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1099,7 +1111,7 @@
       <c r="E31" s="1" t="n">
         <v>0.4966101694915255</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="F31" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1119,7 +1131,7 @@
       <c r="E32" s="1" t="n">
         <v>0.5118644067796611</v>
       </c>
-      <c r="F32" s="1" t="s">
+      <c r="F32" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1139,7 +1151,7 @@
       <c r="E33" s="1" t="n">
         <v>0.5271186440677966</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="F33" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1159,7 +1171,7 @@
       <c r="E34" s="1" t="n">
         <v>0.5423728813559322</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="F34" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1179,7 +1191,7 @@
       <c r="E35" s="1" t="n">
         <v>0.5576271186440678</v>
       </c>
-      <c r="F35" s="1" t="s">
+      <c r="F35" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1199,7 +1211,7 @@
       <c r="E36" s="1" t="n">
         <v>0.5728813559322035</v>
       </c>
-      <c r="F36" s="1" t="s">
+      <c r="F36" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1219,7 +1231,7 @@
       <c r="E37" s="1" t="n">
         <v>0.588135593220339</v>
       </c>
-      <c r="F37" s="1" t="s">
+      <c r="F37" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1239,7 +1251,7 @@
       <c r="E38" s="1" t="n">
         <v>0.6033898305084746</v>
       </c>
-      <c r="F38" s="1" t="s">
+      <c r="F38" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1259,7 +1271,7 @@
       <c r="E39" s="1" t="n">
         <v>0.6186440677966102</v>
       </c>
-      <c r="F39" s="1" t="s">
+      <c r="F39" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1279,7 +1291,7 @@
       <c r="E40" s="1" t="n">
         <v>0.6338983050847458</v>
       </c>
-      <c r="F40" s="1" t="s">
+      <c r="F40" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1299,7 +1311,7 @@
       <c r="E41" s="1" t="n">
         <v>0.6491525423728813</v>
       </c>
-      <c r="F41" s="1" t="s">
+      <c r="F41" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1319,7 +1331,7 @@
       <c r="E42" s="1" t="n">
         <v>0.6644067796610169</v>
       </c>
-      <c r="F42" s="1" t="s">
+      <c r="F42" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1339,7 +1351,7 @@
       <c r="E43" s="1" t="n">
         <v>0.6796610169491526</v>
       </c>
-      <c r="F43" s="1" t="s">
+      <c r="F43" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1359,7 +1371,7 @@
       <c r="E44" s="1" t="n">
         <v>0.6949152542372882</v>
       </c>
-      <c r="F44" s="1" t="s">
+      <c r="F44" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1379,7 +1391,7 @@
       <c r="E45" s="1" t="n">
         <v>0.7101694915254237</v>
       </c>
-      <c r="F45" s="1" t="s">
+      <c r="F45" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1399,7 +1411,7 @@
       <c r="E46" s="1" t="n">
         <v>0.7254237288135593</v>
       </c>
-      <c r="F46" s="1" t="s">
+      <c r="F46" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1419,7 +1431,7 @@
       <c r="E47" s="1" t="n">
         <v>0.7406779661016949</v>
       </c>
-      <c r="F47" s="1" t="s">
+      <c r="F47" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1439,7 +1451,7 @@
       <c r="E48" s="1" t="n">
         <v>0.7559322033898305</v>
       </c>
-      <c r="F48" s="1" t="s">
+      <c r="F48" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1459,7 +1471,7 @@
       <c r="E49" s="1" t="n">
         <v>0.7711864406779662</v>
       </c>
-      <c r="F49" s="1" t="s">
+      <c r="F49" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1479,7 +1491,7 @@
       <c r="E50" s="1" t="n">
         <v>0.7864406779661017</v>
       </c>
-      <c r="F50" s="1" t="s">
+      <c r="F50" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1499,7 +1511,7 @@
       <c r="E51" s="1" t="n">
         <v>0.8016949152542373</v>
       </c>
-      <c r="F51" s="1" t="s">
+      <c r="F51" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1519,7 +1531,7 @@
       <c r="E52" s="1" t="n">
         <v>0.8169491525423729</v>
       </c>
-      <c r="F52" s="1" t="s">
+      <c r="F52" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1539,7 +1551,7 @@
       <c r="E53" s="1" t="n">
         <v>0.8322033898305085</v>
       </c>
-      <c r="F53" s="1" t="s">
+      <c r="F53" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1559,7 +1571,7 @@
       <c r="E54" s="1" t="n">
         <v>0.847457627118644</v>
       </c>
-      <c r="F54" s="1" t="s">
+      <c r="F54" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1579,7 +1591,7 @@
       <c r="E55" s="1" t="n">
         <v>0.8627118644067797</v>
       </c>
-      <c r="F55" s="1" t="s">
+      <c r="F55" s="5" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1599,7 +1611,7 @@
       <c r="E56" s="1" t="n">
         <v>0.8779661016949153</v>
       </c>
-      <c r="F56" s="1" t="s">
+      <c r="F56" s="5" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1619,7 +1631,7 @@
       <c r="E57" s="1" t="n">
         <v>0.8932203389830509</v>
       </c>
-      <c r="F57" s="1" t="s">
+      <c r="F57" s="5" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1639,7 +1651,7 @@
       <c r="E58" s="1" t="n">
         <v>0.9084745762711864</v>
       </c>
-      <c r="F58" s="1" t="s">
+      <c r="F58" s="5" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1659,7 +1671,7 @@
       <c r="E59" s="1" t="n">
         <v>0.923728813559322</v>
       </c>
-      <c r="F59" s="1" t="s">
+      <c r="F59" s="5" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1679,7 +1691,7 @@
       <c r="E60" s="1" t="n">
         <v>0.9389830508474576</v>
       </c>
-      <c r="F60" s="1" t="s">
+      <c r="F60" s="5" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1699,7 +1711,7 @@
       <c r="E61" s="1" t="n">
         <v>0.9542372881355933</v>
       </c>
-      <c r="F61" s="1" t="s">
+      <c r="F61" s="5" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1719,7 +1731,7 @@
       <c r="E62" s="1" t="n">
         <v>0.9694915254237289</v>
       </c>
-      <c r="F62" s="1" t="s">
+      <c r="F62" s="5" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1739,7 +1751,7 @@
       <c r="E63" s="1" t="n">
         <v>0.9847457627118644</v>
       </c>
-      <c r="F63" s="1" t="s">
+      <c r="F63" s="5" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1759,7 +1771,7 @@
       <c r="E64" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F64" s="1" t="s">
+      <c r="F64" s="5" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>